<commit_message>
Example 2 numerical experiments new addition including svd analysis and rearragned unnecessary files
</commit_message>
<xml_diff>
--- a/Examples/Example_2_pendulum/pendulum_data_requirement.xlsx
+++ b/Examples/Example_2_pendulum/pendulum_data_requirement.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manujayadharan/git_repos/DAE-FINDER_dev/Examples/Example_2_pendulum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E14EF69-D8E4-AA43-935D-79190C058B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48EE1E9-C7E7-6C4F-94B3-FB41231A6060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="1720" windowWidth="28040" windowHeight="17440" xr2:uid="{9EB8D5E8-50CE-4E4A-AA48-6024E223E165}"/>
+    <workbookView xWindow="1980" yWindow="1720" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{9EB8D5E8-50CE-4E4A-AA48-6024E223E165}"/>
   </bookViews>
   <sheets>
     <sheet name="Pendulum_Algebraic" sheetId="1" r:id="rId1"/>
     <sheet name="Pendulum_Dynamic" sheetId="2" r:id="rId2"/>
+    <sheet name="Double Pendulum algebraic" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="FrameRate">Pendulum_Algebraic!$G$3</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="9">
   <si>
     <t>Polynomial Degree</t>
   </si>
@@ -61,6 +62,12 @@
   </si>
   <si>
     <t># library terms</t>
+  </si>
+  <si>
+    <t>Total time</t>
+  </si>
+  <si>
+    <t>3mins</t>
   </si>
 </sst>
 </file>
@@ -441,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1784830D-3226-804B-8981-F386CF16A00E}">
   <dimension ref="A2:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -736,4 +743,140 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD27239-841C-7A45-82AC-E03CEE3A1CFD}">
+  <dimension ref="A2:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <f>B3/FrameRate</f>
+        <v>0.21666666666666667</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>60</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <f>B4/FrameRate</f>
+        <v>0.21666666666666667</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>34</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>35</v>
+      </c>
+      <c r="C5">
+        <f>B5/FrameRate</f>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>69</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>39</v>
+      </c>
+      <c r="C6">
+        <f>B6/FrameRate</f>
+        <v>0.65</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>125</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
replaced the chaotic double pendulum with lower resolution for uploading to github
</commit_message>
<xml_diff>
--- a/Examples/Example_2_pendulum/pendulum_data_requirement.xlsx
+++ b/Examples/Example_2_pendulum/pendulum_data_requirement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manujayadharan/git_repos/DAE-FINDER_dev/Examples/Example_2_pendulum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48EE1E9-C7E7-6C4F-94B3-FB41231A6060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2B5FDD-F5D2-8C41-9575-E60A3D45743B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1980" yWindow="1720" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{9EB8D5E8-50CE-4E4A-AA48-6024E223E165}"/>
   </bookViews>
@@ -750,7 +750,7 @@
   <dimension ref="A2:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added pendulum experimental data and plots
</commit_message>
<xml_diff>
--- a/Examples/Example_2_pendulum/pendulum_data_requirement.xlsx
+++ b/Examples/Example_2_pendulum/pendulum_data_requirement.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manujayadharan/git_repos/DAE-FINDER_dev/Examples/Example_2_pendulum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2B5FDD-F5D2-8C41-9575-E60A3D45743B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9C7F21-FA88-0C47-9C68-1597BB39078C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="1720" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{9EB8D5E8-50CE-4E4A-AA48-6024E223E165}"/>
+    <workbookView xWindow="1980" yWindow="1720" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{9EB8D5E8-50CE-4E4A-AA48-6024E223E165}"/>
   </bookViews>
   <sheets>
     <sheet name="Pendulum_Algebraic" sheetId="1" r:id="rId1"/>
     <sheet name="Pendulum_Dynamic" sheetId="2" r:id="rId2"/>
     <sheet name="Double Pendulum algebraic" sheetId="3" r:id="rId3"/>
+    <sheet name="Pendulum experiment video" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="FrameRate">Pendulum_Algebraic!$G$3</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
   <si>
     <t>Polynomial Degree</t>
   </si>
@@ -68,6 +69,21 @@
   </si>
   <si>
     <t>3mins</t>
+  </si>
+  <si>
+    <t>num data points: Algebraic</t>
+  </si>
+  <si>
+    <t>num data points: dynamic</t>
+  </si>
+  <si>
+    <t>&lt;150</t>
+  </si>
+  <si>
+    <t># algebraic library terms</t>
+  </si>
+  <si>
+    <t># dynamic library terms</t>
   </si>
 </sst>
 </file>
@@ -616,7 +632,7 @@
         <v>60</v>
       </c>
       <c r="C3">
-        <f>B3/FrameRate</f>
+        <f t="shared" ref="C3:C9" si="0">B3/FrameRate</f>
         <v>1</v>
       </c>
       <c r="D3">
@@ -640,7 +656,7 @@
         <v>60</v>
       </c>
       <c r="C4">
-        <f>B4/FrameRate</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D4">
@@ -658,7 +674,7 @@
         <v>70</v>
       </c>
       <c r="C5">
-        <f>B5/FrameRate</f>
+        <f t="shared" si="0"/>
         <v>1.1666666666666667</v>
       </c>
       <c r="D5">
@@ -676,7 +692,7 @@
         <v>70</v>
       </c>
       <c r="C6">
-        <f>B6/FrameRate</f>
+        <f t="shared" si="0"/>
         <v>1.1666666666666667</v>
       </c>
       <c r="D6">
@@ -694,7 +710,7 @@
         <v>70</v>
       </c>
       <c r="C7">
-        <f>B7/FrameRate</f>
+        <f t="shared" si="0"/>
         <v>1.1666666666666667</v>
       </c>
       <c r="D7">
@@ -712,7 +728,7 @@
         <v>80</v>
       </c>
       <c r="C8">
-        <f>B8/FrameRate</f>
+        <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="D8">
@@ -730,7 +746,7 @@
         <v>80</v>
       </c>
       <c r="C9">
-        <f>B9/FrameRate</f>
+        <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="D9">
@@ -749,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD27239-841C-7A45-82AC-E03CEE3A1CFD}">
   <dimension ref="A2:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -879,4 +895,90 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261FBDE7-A58B-DA44-9322-40D5DD8170D7}">
+  <dimension ref="A2:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <f>B3/FrameRate</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>9</v>
+      </c>
+      <c r="G3">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>120</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added plots for example 2
</commit_message>
<xml_diff>
--- a/Examples/Example_2_pendulum/pendulum_data_requirement.xlsx
+++ b/Examples/Example_2_pendulum/pendulum_data_requirement.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manujayadharan/git_repos/DAE-FINDER_dev/Examples/Example_2_pendulum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9C7F21-FA88-0C47-9C68-1597BB39078C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4CC311-2E46-A94B-95C5-BFE2A7B3524D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="1720" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{9EB8D5E8-50CE-4E4A-AA48-6024E223E165}"/>
+    <workbookView xWindow="1980" yWindow="1720" windowWidth="28040" windowHeight="17440" xr2:uid="{9EB8D5E8-50CE-4E4A-AA48-6024E223E165}"/>
   </bookViews>
   <sheets>
-    <sheet name="Pendulum_Algebraic" sheetId="1" r:id="rId1"/>
-    <sheet name="Pendulum_Dynamic" sheetId="2" r:id="rId2"/>
+    <sheet name="Pendulum Algebraic" sheetId="1" r:id="rId1"/>
+    <sheet name="Pendulum Dynamic" sheetId="2" r:id="rId2"/>
     <sheet name="Double Pendulum algebraic" sheetId="3" r:id="rId3"/>
     <sheet name="Pendulum experiment video" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="FrameRate">Pendulum_Algebraic!$G$3</definedName>
+    <definedName name="FrameRate">'Pendulum Algebraic'!$G$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -462,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1784830D-3226-804B-8981-F386CF16A00E}">
-  <dimension ref="A2:Q17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,104 +476,104 @@
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="A2">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <f>B2/FrameRate</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
         <v>5</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="G2">
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C3">
         <f>B3/FrameRate</f>
-        <v>0.16666666666666666</v>
+        <v>0.38333333333333336</v>
       </c>
       <c r="D3">
         <v>4</v>
       </c>
       <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>0.5</v>
-      </c>
-      <c r="G3">
-        <v>60</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="C4">
         <f>B4/FrameRate</f>
-        <v>0.38333333333333336</v>
+        <v>0.65</v>
       </c>
       <c r="D4">
         <v>4</v>
       </c>
       <c r="E4">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>39</v>
+        <v>165</v>
       </c>
       <c r="C5">
         <f>B5/FrameRate</f>
-        <v>0.65</v>
+        <v>2.75</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>165</v>
-      </c>
-      <c r="C6">
-        <f>B6/FrameRate</f>
-        <v>2.75</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
         <v>20</v>
       </c>
     </row>
@@ -593,82 +593,101 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C1F16B-90AA-9B4F-B115-062FD90DB919}">
-  <dimension ref="A2:G9"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>60</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C8" si="0">B2/FrameRate</f>
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="G2">
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>60</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C9" si="0">B3/FrameRate</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D3">
         <v>4</v>
       </c>
       <c r="E3">
-        <v>7</v>
-      </c>
-      <c r="F3">
-        <v>0.5</v>
-      </c>
-      <c r="G3">
-        <v>60</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="D4">
         <v>4</v>
       </c>
       <c r="E4">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>70</v>
@@ -681,12 +700,12 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>70</v>
@@ -699,30 +718,30 @@
         <v>4</v>
       </c>
       <c r="E6">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>1.1666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="D7">
         <v>4</v>
       </c>
       <c r="E7">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>80</v>
@@ -734,25 +753,7 @@
       <c r="D8">
         <v>4</v>
       </c>
-      <c r="E8">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>80</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="D9">
-        <v>4</v>
-      </c>
-      <c r="E9" s="1">
+      <c r="E8" s="1">
         <v>46</v>
       </c>
     </row>
@@ -763,48 +764,76 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD27239-841C-7A45-82AC-E03CEE3A1CFD}">
-  <dimension ref="A2:H6"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H10"/>
+      <selection sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <f>B2/FrameRate</f>
+        <v>0.21666666666666667</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>14</v>
+      </c>
+      <c r="F2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
+      <c r="G2">
+        <v>60</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>13</v>
@@ -817,34 +846,28 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3">
-        <v>60</v>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C4">
         <f>B4/FrameRate</f>
-        <v>0.21666666666666667</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -852,43 +875,22 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C5">
         <f>B5/FrameRate</f>
-        <v>0.58333333333333337</v>
+        <v>0.65</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>69</v>
+        <v>125</v>
       </c>
       <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>39</v>
-      </c>
-      <c r="C6">
-        <f>B6/FrameRate</f>
-        <v>0.65</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>125</v>
-      </c>
-      <c r="F6">
         <v>0</v>
       </c>
     </row>
@@ -899,10 +901,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261FBDE7-A58B-DA44-9322-40D5DD8170D7}">
-  <dimension ref="A2:J3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -913,68 +915,68 @@
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <f>B2/FrameRate</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>9</v>
+      </c>
+      <c r="G2">
+        <v>11</v>
+      </c>
+      <c r="H2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" t="s">
-        <v>5</v>
+      <c r="I2">
+        <v>120</v>
       </c>
       <c r="J2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>200</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <f>B3/FrameRate</f>
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>9</v>
-      </c>
-      <c r="G3">
-        <v>11</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>120</v>
-      </c>
-      <c r="J3" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>